<commit_message>
chore: Update roles data structure in CSV and XLSX files to include permissions and metadata for enhanced role management
</commit_message>
<xml_diff>
--- a/seeds/roles.xlsx
+++ b/seeds/roles.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="45">
   <si>
     <t>role_id</t>
   </si>
@@ -59,6 +59,12 @@
     <t>icon</t>
   </si>
   <si>
+    <t>permissions</t>
+  </si>
+  <si>
+    <t>metadata</t>
+  </si>
+  <si>
     <t>admin</t>
   </si>
   <si>
@@ -74,6 +80,12 @@
     <t>icon-shield</t>
   </si>
   <si>
+    <t>{"users":["create","read","update","delete"],"roles":["create","read","update","delete"]}</t>
+  </si>
+  <si>
+    <t>{"max_users":5,"requires_approval":true}</t>
+  </si>
+  <si>
     <t>moderator</t>
   </si>
   <si>
@@ -89,6 +101,12 @@
     <t>icon-user-check</t>
   </si>
   <si>
+    <t>{"users":["read","update"],"content":["create","read","update","delete"]}</t>
+  </si>
+  <si>
+    <t>{"max_users":0}</t>
+  </si>
+  <si>
     <t>editor</t>
   </si>
   <si>
@@ -104,6 +122,9 @@
     <t>icon-edit</t>
   </si>
   <si>
+    <t>{"content":["create","read","update"]}</t>
+  </si>
+  <si>
     <t>viewer</t>
   </si>
   <si>
@@ -119,6 +140,12 @@
     <t>icon-eye</t>
   </si>
   <si>
+    <t>{"content":["read"]}</t>
+  </si>
+  <si>
+    <t>{}</t>
+  </si>
+  <si>
     <t>guest</t>
   </si>
   <si>
@@ -132,6 +159,9 @@
   </si>
   <si>
     <t>icon-user</t>
+  </si>
+  <si>
+    <t>{"max_sessions":1,"session_timeout":3600}</t>
   </si>
 </sst>
 </file>
@@ -1284,7 +1314,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleSheetLayoutView="60" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1292,7 +1322,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.3846153846154" defaultRowHeight="16.8" outlineLevelRow="5"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1323,16 +1353,22 @@
       <c r="J1" t="s">
         <v>9</v>
       </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D2">
         <v>100</v>
@@ -1350,21 +1386,27 @@
         <v>1</v>
       </c>
       <c r="I2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="J2" t="s">
-        <v>14</v>
+        <v>16</v>
+      </c>
+      <c r="K2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" t="s">
+        <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D3">
         <v>50</v>
@@ -1382,21 +1424,27 @@
         <v>2</v>
       </c>
       <c r="I3" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="J3" t="s">
-        <v>19</v>
+        <v>23</v>
+      </c>
+      <c r="K3" t="s">
+        <v>24</v>
+      </c>
+      <c r="L3" t="s">
+        <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:12">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="D4">
         <v>30</v>
@@ -1414,21 +1462,27 @@
         <v>3</v>
       </c>
       <c r="I4" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="J4" t="s">
-        <v>24</v>
+        <v>30</v>
+      </c>
+      <c r="K4" t="s">
+        <v>31</v>
+      </c>
+      <c r="L4" t="s">
+        <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:12">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="D5">
         <v>10</v>
@@ -1446,21 +1500,27 @@
         <v>4</v>
       </c>
       <c r="I5" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="J5" t="s">
-        <v>29</v>
+        <v>36</v>
+      </c>
+      <c r="K5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L5" t="s">
+        <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:12">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="C6" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="D6">
         <v>5</v>
@@ -1478,10 +1538,16 @@
         <v>5</v>
       </c>
       <c r="I6" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="J6" t="s">
-        <v>34</v>
+        <v>43</v>
+      </c>
+      <c r="K6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L6" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>